<commit_message>
Avoiding cartesian joins within income_tax Export pminV
</commit_message>
<xml_diff>
--- a/data-raw/medicare-tables.xlsx
+++ b/data-raw/medicare-tables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romanesd\Documents\GitHub\rgrattan\grattan\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romanesd\Documents\GitHub\rgrattan\grattan\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
   <si>
     <t>fy_year</t>
   </si>
@@ -86,6 +86,18 @@
   </si>
   <si>
     <t>2015-16</t>
+  </si>
+  <si>
+    <t>2005-06</t>
+  </si>
+  <si>
+    <t>2004-05</t>
+  </si>
+  <si>
+    <t>2003-04</t>
+  </si>
+  <si>
+    <t>http://www.budget.gov.au/2005-06/bp1/download/bp1_bst5.pdf</t>
   </si>
 </sst>
 </file>
@@ -455,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,10 +1043,10 @@
         <v>0</v>
       </c>
       <c r="D25" s="1">
-        <v>16740</v>
+        <v>15902</v>
       </c>
       <c r="E25" s="1">
-        <v>19694</v>
+        <v>17191</v>
       </c>
       <c r="F25" s="3">
         <v>0.1</v>
@@ -1086,6 +1098,75 @@
         <v>0.1</v>
       </c>
       <c r="G27">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>15903</v>
+      </c>
+      <c r="E28" s="1">
+        <v>17191</v>
+      </c>
+      <c r="F28" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G28">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" t="b">
+        <v>0</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>15903</v>
+      </c>
+      <c r="E29" s="1">
+        <v>17191</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G29">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>15530</v>
+      </c>
+      <c r="E30" s="1">
+        <v>16788</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G30">
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
@@ -1271,9 +1352,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1282,6 +1365,11 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
The Act (previous commit) had assumed contemporaneous parameters.
`new_medicare_levy` = `medicare_levy`
</commit_message>
<xml_diff>
--- a/data-raw/medicare-tables.xlsx
+++ b/data-raw/medicare-tables.xlsx
@@ -494,7 +494,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,16 +566,25 @@
         <v>23</v>
       </c>
       <c r="F2" s="1">
-        <v>15530</v>
+        <v>15529</v>
       </c>
       <c r="G2" s="1">
-        <v>16788</v>
+        <v>16789</v>
       </c>
       <c r="H2" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I2">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>26205</v>
+      </c>
+      <c r="K2" s="1">
+        <v>26206</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2406</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -595,16 +604,25 @@
         <v>23</v>
       </c>
       <c r="F3" s="1">
-        <v>15903</v>
+        <v>15902</v>
       </c>
       <c r="G3" s="1">
-        <v>17191</v>
+        <v>17192</v>
       </c>
       <c r="H3" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I3">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J3" s="1">
+        <v>26834</v>
+      </c>
+      <c r="K3" s="1">
+        <v>26835</v>
+      </c>
+      <c r="L3" s="1">
+        <v>2464</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -624,16 +642,25 @@
         <v>23</v>
       </c>
       <c r="F4" s="1">
-        <v>15903</v>
+        <v>16284</v>
       </c>
       <c r="G4" s="1">
-        <v>17191</v>
+        <v>17605</v>
       </c>
       <c r="H4" s="3">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="I4">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>27478</v>
+      </c>
+      <c r="K4" s="1">
+        <v>27479</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2523</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -653,16 +680,25 @@
         <v>23</v>
       </c>
       <c r="F5" s="1">
-        <v>15902</v>
+        <v>16740</v>
       </c>
       <c r="G5" s="1">
-        <v>17191</v>
+        <v>19695</v>
       </c>
       <c r="H5" s="3">
         <v>0.1</v>
       </c>
       <c r="I5">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>28247</v>
+      </c>
+      <c r="K5" s="1">
+        <v>28248</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2594</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -693,6 +729,15 @@
       <c r="I6">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="J6" s="1">
+        <v>33500</v>
+      </c>
+      <c r="K6" s="1">
+        <v>33501</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2594</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -721,6 +766,15 @@
       </c>
       <c r="I7">
         <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>33500</v>
+      </c>
+      <c r="K7" s="1">
+        <v>33501</v>
+      </c>
+      <c r="L7" s="1">
+        <v>2594</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update sysdata for s8(5) of Act
</commit_message>
<xml_diff>
--- a/data-raw/medicare-tables.xlsx
+++ b/data-raw/medicare-tables.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hugh Parsonage\Documents\Github\grattan\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughp\Documents\grattan\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -515,8 +515,8 @@
   <dimension ref="A1:L54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,13 +680,13 @@
         <v>0.02</v>
       </c>
       <c r="J4" s="1">
-        <v>36001</v>
+        <v>35261</v>
       </c>
       <c r="K4" s="1">
         <v>44077</v>
       </c>
       <c r="L4" s="1">
-        <v>3306</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -726,7 +726,7 @@
         <v>57501</v>
       </c>
       <c r="L5" s="1">
-        <v>3306</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
More thorough check for #50
Checked Budget Paper No. 2
</commit_message>
<xml_diff>
--- a/data-raw/medicare-tables.xlsx
+++ b/data-raw/medicare-tables.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="37">
   <si>
     <t>fy_year</t>
   </si>
@@ -97,9 +97,6 @@
     <t>family_status</t>
   </si>
   <si>
-    <t>individual</t>
-  </si>
-  <si>
     <t>family</t>
   </si>
   <si>
@@ -136,13 +133,10 @@
     <t>1999-00</t>
   </si>
   <si>
-    <t>Spouse without dependant child or student child</t>
-  </si>
-  <si>
-    <t>Spouse with one dependant child</t>
-  </si>
-  <si>
-    <t>Spouse with more than one dependant child</t>
+    <t>http://budget.gov.au/2015-16/content/bp2/download/BP2_consolidated.pdf</t>
+  </si>
+  <si>
+    <t>p. 26 (p. 42 in PDF)</t>
   </si>
 </sst>
 </file>
@@ -512,28 +506,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -544,36 +537,33 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" t="s">
-        <v>2</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="b">
         <f>D2</f>
@@ -585,77 +575,74 @@
       <c r="D2" t="b">
         <v>0</v>
       </c>
-      <c r="E2" t="s">
-        <v>23</v>
+      <c r="E2" s="1">
+        <v>21335</v>
       </c>
       <c r="F2" s="1">
-        <v>21335</v>
-      </c>
-      <c r="G2" s="1">
-        <v>26668</v>
-      </c>
-      <c r="H2" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I2" s="2">
+        <f t="shared" ref="F2:F39" si="0">ROUND((E2 +1)*G2/(G2-H2), 0)</f>
+        <v>26670</v>
+      </c>
+      <c r="G2" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="2">
         <v>0.02</v>
       </c>
+      <c r="I2" s="1">
+        <v>36001</v>
+      </c>
       <c r="J2" s="1">
-        <v>36001</v>
+        <v>44077</v>
       </c>
       <c r="K2" s="1">
-        <v>44077</v>
-      </c>
-      <c r="L2" s="1">
         <v>3306</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="b">
-        <f t="shared" ref="B3:B11" si="0">D3</f>
+        <f t="shared" ref="B3:B11" si="1">D3</f>
         <v>1</v>
       </c>
       <c r="C3" t="b">
-        <f t="shared" ref="C3:C11" si="1">NOT(D3)</f>
+        <f t="shared" ref="C3:C11" si="2">NOT(D3)</f>
         <v>0</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
-        <v>23</v>
+      <c r="E3" s="1">
+        <v>33738</v>
       </c>
       <c r="F3" s="1">
-        <v>33738</v>
-      </c>
-      <c r="G3" s="1">
-        <v>41306</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I3" s="2">
+        <f t="shared" si="0"/>
+        <v>42174</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H3" s="2">
         <v>0.02</v>
       </c>
+      <c r="I3" s="1">
+        <v>46966</v>
+      </c>
       <c r="J3" s="1">
-        <v>46966</v>
+        <f>ROUND((I3 +1)*G3/(G3-H3), 0)</f>
+        <v>58709</v>
       </c>
       <c r="K3" s="1">
-        <v>57501</v>
-      </c>
-      <c r="L3" s="1">
         <v>3306</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C4" t="b">
@@ -664,77 +651,75 @@
       <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
+      <c r="E4" s="1">
+        <v>20896</v>
       </c>
       <c r="F4" s="1">
-        <v>21335</v>
-      </c>
-      <c r="G4" s="1">
-        <v>26668</v>
-      </c>
-      <c r="H4" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>26121</v>
+      </c>
+      <c r="G4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H4" s="2">
         <v>0.02</v>
       </c>
+      <c r="I4" s="1">
+        <v>35261</v>
+      </c>
       <c r="J4" s="1">
-        <v>35261</v>
+        <f t="shared" ref="J4:J47" si="3">ROUND((I4 +1)*G4/(G4-H4), 0)</f>
+        <v>44078</v>
       </c>
       <c r="K4" s="1">
-        <v>44077</v>
-      </c>
-      <c r="L4" s="1">
         <v>3238</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C5" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>23</v>
+      <c r="E5" s="1">
+        <v>33044</v>
       </c>
       <c r="F5" s="1">
-        <v>33738</v>
-      </c>
-      <c r="G5" s="1">
+        <f t="shared" si="0"/>
         <v>41306</v>
       </c>
-      <c r="H5" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I5" s="2">
+      <c r="G5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="2">
         <v>0.02</v>
       </c>
+      <c r="I5" s="1">
+        <v>46966</v>
+      </c>
       <c r="J5" s="1">
-        <v>46966</v>
+        <f t="shared" si="3"/>
+        <v>58709</v>
       </c>
       <c r="K5" s="1">
-        <v>57501</v>
-      </c>
-      <c r="L5" s="1">
         <v>3238</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C6" t="b">
@@ -743,156 +728,152 @@
       <c r="D6" t="b">
         <v>0</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
+      <c r="E6" s="1">
+        <v>20542</v>
       </c>
       <c r="F6" s="1">
-        <v>20896</v>
-      </c>
-      <c r="G6" s="1">
-        <v>26121</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I6" s="2">
+        <f t="shared" si="0"/>
+        <v>25679</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="2">
         <v>0.02</v>
       </c>
+      <c r="I6" s="1">
+        <v>34367</v>
+      </c>
       <c r="J6" s="1">
-        <v>35261</v>
+        <f t="shared" si="3"/>
+        <v>42960</v>
       </c>
       <c r="K6" s="1">
-        <v>44077</v>
-      </c>
-      <c r="L6" s="1">
-        <v>3238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
       <c r="B7" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C7" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>32279</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>40350</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="I7" s="1">
+        <v>46000</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="3"/>
+        <v>57501</v>
+      </c>
+      <c r="K7" s="1">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="1">
-        <v>33044</v>
-      </c>
-      <c r="G7" s="1">
-        <v>41306</v>
-      </c>
-      <c r="H7" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>20542</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="0"/>
+        <v>24168</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I8" s="1">
+        <v>34367</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="3"/>
+        <v>40433</v>
+      </c>
+      <c r="K8" s="1">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="C9" t="b">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>32279</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
+        <v>37976</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H9">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I9" s="1">
         <v>46000</v>
       </c>
-      <c r="K7" s="1">
-        <v>57501</v>
-      </c>
-      <c r="L7" s="1">
-        <v>3238</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" t="b">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C8" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="1">
-        <v>20542</v>
-      </c>
-      <c r="G8" s="1">
-        <v>24167</v>
-      </c>
-      <c r="H8" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I8">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J8" s="1">
-        <v>34367</v>
-      </c>
-      <c r="K8" s="1">
-        <v>40432</v>
-      </c>
-      <c r="L8" s="1">
+      <c r="J9" s="1">
+        <f t="shared" si="3"/>
+        <v>54119</v>
+      </c>
+      <c r="K9" s="1">
         <v>3156</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" t="b">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="C9" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="1">
-        <v>32279</v>
-      </c>
-      <c r="G9" s="1">
-        <v>37975</v>
-      </c>
-      <c r="H9" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I9">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J9" s="1">
-        <v>46000</v>
-      </c>
-      <c r="K9" s="1">
-        <v>54117</v>
-      </c>
-      <c r="L9" s="1">
-        <v>3156</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C10" t="b">
@@ -901,72 +882,70 @@
       <c r="D10" t="b">
         <v>0</v>
       </c>
-      <c r="E10" t="s">
-        <v>23</v>
+      <c r="E10" s="1">
+        <v>20542</v>
       </c>
       <c r="F10" s="1">
-        <v>20542</v>
-      </c>
-      <c r="G10" s="1">
+        <f t="shared" si="0"/>
         <v>24168</v>
       </c>
-      <c r="H10" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I10">
-        <v>1.4999999999999999E-2</v>
+      <c r="G10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I10" s="1">
+        <v>33693</v>
       </c>
       <c r="J10" s="1">
-        <v>33693</v>
+        <f t="shared" si="3"/>
+        <v>39640</v>
       </c>
       <c r="K10" s="1">
-        <v>39639</v>
-      </c>
-      <c r="L10" s="1">
         <v>3094</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="C11" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>23</v>
+      <c r="E11" s="1">
+        <v>32279</v>
       </c>
       <c r="F11" s="1">
-        <v>32279</v>
-      </c>
-      <c r="G11" s="1">
-        <v>37975</v>
-      </c>
-      <c r="H11" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I11">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>37976</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H11">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I11" s="1">
+        <v>46000</v>
       </c>
       <c r="J11" s="1">
-        <v>46000</v>
+        <f t="shared" si="3"/>
+        <v>54119</v>
       </c>
       <c r="K11" s="1">
-        <v>54117</v>
-      </c>
-      <c r="L11" s="1">
         <v>3094</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -979,32 +958,31 @@
       <c r="D12" t="b">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
-        <v>23</v>
+      <c r="E12" s="1">
+        <v>19404</v>
       </c>
       <c r="F12" s="1">
-        <v>19404</v>
-      </c>
-      <c r="G12" s="1">
-        <v>22828</v>
-      </c>
-      <c r="H12" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I12">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>22829</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H12">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I12" s="1">
+        <v>32743</v>
       </c>
       <c r="J12" s="1">
-        <v>32743</v>
+        <f t="shared" si="3"/>
+        <v>38522</v>
       </c>
       <c r="K12" s="1">
-        <v>38522</v>
-      </c>
-      <c r="L12" s="1">
         <v>3007</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1017,32 +995,31 @@
       <c r="D13" t="b">
         <v>0</v>
       </c>
-      <c r="E13" t="s">
-        <v>23</v>
+      <c r="E13" s="1">
+        <v>30452</v>
       </c>
       <c r="F13" s="1">
-        <v>30452</v>
-      </c>
-      <c r="G13" s="1">
-        <v>35824</v>
-      </c>
-      <c r="H13" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I13">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>35827</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H13">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I13" s="1">
+        <v>32743</v>
       </c>
       <c r="J13" s="1">
-        <v>32743</v>
+        <f t="shared" si="3"/>
+        <v>38522</v>
       </c>
       <c r="K13" s="1">
-        <v>38522</v>
-      </c>
-      <c r="L13" s="1">
         <v>3007</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1055,29 +1032,31 @@
       <c r="D14" t="b">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>23</v>
+      <c r="E14" s="1">
+        <v>30685</v>
       </c>
       <c r="F14" s="1">
-        <v>30685</v>
-      </c>
-      <c r="G14" s="1">
-        <v>36100</v>
-      </c>
-      <c r="H14" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I14">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>36101</v>
+      </c>
+      <c r="G14" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H14">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I14" s="1">
+        <v>44500</v>
       </c>
       <c r="J14" s="1">
-        <v>44500</v>
-      </c>
-      <c r="L14" s="1">
+        <f t="shared" si="3"/>
+        <v>52354</v>
+      </c>
+      <c r="K14" s="1">
         <v>3007</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1090,32 +1069,31 @@
       <c r="D15" t="b">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>23</v>
+      <c r="E15" s="1">
+        <v>18839</v>
       </c>
       <c r="F15" s="1">
-        <v>18839</v>
-      </c>
-      <c r="G15" s="1">
-        <v>22163</v>
-      </c>
-      <c r="H15" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I15">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>22165</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H15">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I15" s="1">
+        <v>31789</v>
       </c>
       <c r="J15" s="1">
-        <v>31789</v>
+        <f t="shared" si="3"/>
+        <v>37400</v>
       </c>
       <c r="K15" s="1">
-        <v>37399</v>
-      </c>
-      <c r="L15" s="1">
         <v>2919</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1128,26 +1106,24 @@
       <c r="D16" t="b">
         <v>0</v>
       </c>
-      <c r="E16" t="s">
-        <v>23</v>
+      <c r="E16" s="1">
+        <v>30439</v>
       </c>
       <c r="F16" s="1">
-        <v>30439</v>
-      </c>
-      <c r="G16" s="1">
-        <v>35811</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I16">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="L16" s="1">
+        <f t="shared" si="0"/>
+        <v>35812</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H16">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K16" s="1">
         <v>2919</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1160,29 +1136,31 @@
       <c r="D17" t="b">
         <v>1</v>
       </c>
-      <c r="E17" t="s">
-        <v>23</v>
+      <c r="E17" s="1">
+        <v>30685</v>
       </c>
       <c r="F17" s="1">
-        <v>30685</v>
-      </c>
-      <c r="G17" s="1">
-        <v>36100</v>
-      </c>
-      <c r="H17" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I17">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>36101</v>
+      </c>
+      <c r="G17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H17">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <v>44500</v>
       </c>
       <c r="J17" s="1">
-        <v>44500</v>
-      </c>
-      <c r="L17" s="1">
+        <f t="shared" si="3"/>
+        <v>52354</v>
+      </c>
+      <c r="K17" s="1">
         <v>2919</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1195,32 +1173,31 @@
       <c r="D18" t="b">
         <v>0</v>
       </c>
-      <c r="E18" t="s">
-        <v>23</v>
+      <c r="E18" s="1">
+        <v>18488</v>
       </c>
       <c r="F18" s="1">
-        <v>18488</v>
-      </c>
-      <c r="G18" s="1">
-        <v>21750</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I18">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>21752</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I18" s="1">
+        <v>31196</v>
       </c>
       <c r="J18" s="1">
-        <v>31196</v>
+        <f t="shared" si="3"/>
+        <v>36702</v>
       </c>
       <c r="K18" s="1">
-        <v>36702</v>
-      </c>
-      <c r="L18" s="1">
         <v>2865</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -1233,26 +1210,24 @@
       <c r="D19" t="b">
         <v>0</v>
       </c>
-      <c r="E19" t="s">
-        <v>23</v>
+      <c r="E19" s="1">
+        <v>27697</v>
       </c>
       <c r="F19" s="1">
-        <v>27697</v>
-      </c>
-      <c r="G19" s="1">
-        <v>32584</v>
-      </c>
-      <c r="H19" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I19">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="L19" s="1">
+        <f t="shared" si="0"/>
+        <v>32586</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H19">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K19" s="1">
         <v>2865</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -1265,29 +1240,31 @@
       <c r="D20" t="b">
         <v>1</v>
       </c>
-      <c r="E20" t="s">
-        <v>23</v>
+      <c r="E20" s="1">
+        <v>29867</v>
       </c>
       <c r="F20" s="1">
-        <v>29867</v>
-      </c>
-      <c r="G20" s="1">
-        <v>35137</v>
-      </c>
-      <c r="H20" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I20">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>35139</v>
+      </c>
+      <c r="G20" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H20">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I20" s="1">
+        <v>43500</v>
       </c>
       <c r="J20" s="1">
-        <v>43500</v>
-      </c>
-      <c r="L20" s="1">
+        <f t="shared" si="3"/>
+        <v>51178</v>
+      </c>
+      <c r="K20" s="1">
         <v>2865</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1300,32 +1277,31 @@
       <c r="D21" t="b">
         <v>0</v>
       </c>
-      <c r="E21" t="s">
-        <v>23</v>
+      <c r="E21" s="1">
+        <v>17794</v>
       </c>
       <c r="F21" s="1">
-        <v>17794</v>
-      </c>
-      <c r="G21" s="1">
-        <v>20934</v>
-      </c>
-      <c r="H21" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I21">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>20935</v>
+      </c>
+      <c r="G21" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H21">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I21" s="1">
+        <v>30025</v>
       </c>
       <c r="J21" s="1">
-        <v>30025</v>
+        <f t="shared" si="3"/>
+        <v>35325</v>
       </c>
       <c r="K21" s="1">
-        <v>35324</v>
-      </c>
-      <c r="L21" s="1">
         <v>2757</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1338,29 +1314,31 @@
       <c r="D22" t="b">
         <v>0</v>
       </c>
-      <c r="E22" t="s">
-        <v>23</v>
+      <c r="E22" s="1">
+        <v>25299</v>
       </c>
       <c r="F22" s="1">
-        <v>25299</v>
-      </c>
-      <c r="G22" s="1">
-        <v>29763</v>
-      </c>
-      <c r="H22" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I22">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>29765</v>
+      </c>
+      <c r="G22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H22">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I22" s="1">
+        <v>42000</v>
       </c>
       <c r="J22" s="1">
-        <v>42000</v>
-      </c>
-      <c r="L22" s="1">
+        <f t="shared" si="3"/>
+        <v>49413</v>
+      </c>
+      <c r="K22" s="1">
         <v>2757</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1373,29 +1351,31 @@
       <c r="D23" t="b">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
-        <v>23</v>
+      <c r="E23" s="1">
+        <v>28867</v>
       </c>
       <c r="F23" s="1">
-        <v>28867</v>
-      </c>
-      <c r="G23" s="1">
-        <v>33961</v>
-      </c>
-      <c r="H23" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I23">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>33962</v>
+      </c>
+      <c r="G23" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H23">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I23" s="1">
+        <v>42000</v>
       </c>
       <c r="J23" s="1">
-        <v>42000</v>
-      </c>
-      <c r="L23" s="1">
+        <f t="shared" si="3"/>
+        <v>49413</v>
+      </c>
+      <c r="K23" s="1">
         <v>2757</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1408,32 +1388,31 @@
       <c r="D24" t="b">
         <v>0</v>
       </c>
-      <c r="E24" t="s">
-        <v>23</v>
+      <c r="E24" s="1">
+        <v>17309</v>
       </c>
       <c r="F24" s="1">
-        <v>17309</v>
-      </c>
-      <c r="G24" s="1">
-        <v>20363</v>
-      </c>
-      <c r="H24" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I24">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>20365</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H24">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>29207</v>
       </c>
       <c r="J24" s="1">
-        <v>29207</v>
+        <f t="shared" si="3"/>
+        <v>34362</v>
       </c>
       <c r="K24" s="1">
-        <v>29208</v>
-      </c>
-      <c r="L24" s="1">
         <v>2682</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -1446,32 +1425,31 @@
       <c r="D25" t="b">
         <v>0</v>
       </c>
-      <c r="E25" t="s">
-        <v>23</v>
+      <c r="E25" s="1">
+        <v>22922</v>
       </c>
       <c r="F25" s="1">
-        <v>22922</v>
-      </c>
-      <c r="G25" s="1">
-        <v>26967</v>
-      </c>
-      <c r="H25" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I25">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>26968</v>
+      </c>
+      <c r="G25" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H25">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I25" s="1">
+        <v>33500</v>
       </c>
       <c r="J25" s="1">
-        <v>33500</v>
+        <f t="shared" si="3"/>
+        <v>39413</v>
       </c>
       <c r="K25" s="1">
-        <v>33501</v>
-      </c>
-      <c r="L25" s="1">
         <v>2682</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -1484,32 +1462,31 @@
       <c r="D26" t="b">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>23</v>
+      <c r="E26" s="1">
+        <v>25867</v>
       </c>
       <c r="F26" s="1">
-        <v>25867</v>
-      </c>
-      <c r="G26" s="1">
-        <v>30431</v>
-      </c>
-      <c r="H26" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I26">
-        <v>1.4999999999999999E-2</v>
+        <f t="shared" si="0"/>
+        <v>30433</v>
+      </c>
+      <c r="G26" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H26">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I26" s="1">
+        <v>33500</v>
       </c>
       <c r="J26" s="1">
-        <v>33500</v>
+        <f t="shared" si="3"/>
+        <v>39413</v>
       </c>
       <c r="K26" s="1">
-        <v>33501</v>
-      </c>
-      <c r="L26" s="1">
         <v>2682</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>12</v>
       </c>
@@ -1522,32 +1499,31 @@
       <c r="D27" t="b">
         <v>0</v>
       </c>
-      <c r="E27" t="s">
-        <v>23</v>
+      <c r="E27" s="1">
+        <v>16740</v>
       </c>
       <c r="F27" s="1">
-        <v>16740</v>
-      </c>
-      <c r="G27" s="1">
+        <f t="shared" si="0"/>
         <v>19695</v>
       </c>
-      <c r="H27" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I27">
-        <v>1.4999999999999999E-2</v>
+      <c r="G27" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H27">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I27" s="1">
+        <v>28247</v>
       </c>
       <c r="J27" s="1">
-        <v>28247</v>
+        <f t="shared" si="3"/>
+        <v>33233</v>
       </c>
       <c r="K27" s="1">
-        <v>28248</v>
-      </c>
-      <c r="L27" s="1">
         <v>2594</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -1560,33 +1536,31 @@
       <c r="D28" t="b">
         <v>0</v>
       </c>
-      <c r="E28" t="s">
-        <v>23</v>
+      <c r="E28" s="1">
+        <v>21637</v>
       </c>
       <c r="F28" s="1">
-        <v>21637</v>
-      </c>
-      <c r="G28" s="1">
-        <f t="shared" ref="G28:G32" si="2">ROUND((F28 +1)*H28/(H28-I28), 0)</f>
+        <f t="shared" si="0"/>
         <v>25456</v>
       </c>
-      <c r="H28" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I28">
-        <v>1.4999999999999999E-2</v>
+      <c r="G28" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H28">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I28" s="1">
+        <v>33500</v>
       </c>
       <c r="J28" s="1">
-        <v>33500</v>
+        <f t="shared" si="3"/>
+        <v>39413</v>
       </c>
       <c r="K28" s="1">
-        <v>33501</v>
-      </c>
-      <c r="L28" s="1">
         <v>2594</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1599,33 +1573,31 @@
       <c r="D29" t="b">
         <v>1</v>
       </c>
-      <c r="E29" t="s">
-        <v>23</v>
+      <c r="E29" s="1">
+        <v>24867</v>
       </c>
       <c r="F29" s="1">
-        <v>24867</v>
-      </c>
-      <c r="G29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>29256</v>
       </c>
-      <c r="H29" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="I29">
-        <v>1.4999999999999999E-2</v>
+      <c r="G29" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="H29">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I29" s="1">
+        <v>33500</v>
       </c>
       <c r="J29" s="1">
-        <v>33500</v>
+        <f t="shared" si="3"/>
+        <v>39413</v>
       </c>
       <c r="K29" s="1">
-        <v>33501</v>
-      </c>
-      <c r="L29" s="1">
         <v>2594</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -1638,33 +1610,31 @@
       <c r="D30" t="b">
         <v>0</v>
       </c>
-      <c r="E30" t="s">
-        <v>23</v>
+      <c r="E30" s="1">
+        <v>16284</v>
       </c>
       <c r="F30" s="1">
-        <v>16284</v>
-      </c>
-      <c r="G30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>17605</v>
       </c>
-      <c r="H30" s="3">
+      <c r="G30" s="3">
         <v>0.2</v>
       </c>
-      <c r="I30">
-        <v>1.4999999999999999E-2</v>
+      <c r="H30">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I30" s="1">
+        <v>27478</v>
       </c>
       <c r="J30" s="1">
-        <v>27478</v>
+        <f t="shared" si="3"/>
+        <v>29707</v>
       </c>
       <c r="K30" s="1">
-        <v>27479</v>
-      </c>
-      <c r="L30" s="1">
         <v>2523</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -1677,33 +1647,31 @@
       <c r="D31" t="b">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
-        <v>23</v>
+      <c r="E31" s="1">
+        <v>21968</v>
       </c>
       <c r="F31" s="1">
-        <v>21968</v>
-      </c>
-      <c r="G31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>23750</v>
       </c>
-      <c r="H31" s="3">
+      <c r="G31" s="3">
         <v>0.2</v>
       </c>
-      <c r="I31">
-        <v>1.4999999999999999E-2</v>
+      <c r="H31">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I31" s="1">
+        <v>31729</v>
       </c>
       <c r="J31" s="1">
-        <v>31729</v>
+        <f t="shared" si="3"/>
+        <v>34303</v>
       </c>
       <c r="K31" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L31" s="1">
         <v>2523</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1716,33 +1684,31 @@
       <c r="D32" t="b">
         <v>0</v>
       </c>
-      <c r="E32" t="s">
-        <v>23</v>
+      <c r="E32" s="1">
+        <v>19583</v>
       </c>
       <c r="F32" s="1">
-        <v>19583</v>
-      </c>
-      <c r="G32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>21172</v>
       </c>
-      <c r="H32" s="3">
+      <c r="G32" s="3">
         <v>0.2</v>
       </c>
-      <c r="I32">
-        <v>1.4999999999999999E-2</v>
+      <c r="H32">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I32" s="1">
+        <v>31729</v>
       </c>
       <c r="J32" s="1">
-        <v>31729</v>
+        <f t="shared" si="3"/>
+        <v>34303</v>
       </c>
       <c r="K32" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L32" s="1">
         <v>2523</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1755,33 +1721,31 @@
       <c r="D33" t="b">
         <v>0</v>
       </c>
-      <c r="E33" t="s">
-        <v>23</v>
+      <c r="E33" s="1">
+        <v>15902</v>
       </c>
       <c r="F33" s="1">
-        <v>15902</v>
-      </c>
-      <c r="G33" s="1">
-        <f t="shared" ref="G33:G36" si="3">ROUND((F33 +1)*H33/(H33-I33), 0)</f>
+        <f t="shared" si="0"/>
         <v>17192</v>
       </c>
-      <c r="H33" s="3">
+      <c r="G33" s="3">
         <v>0.2</v>
       </c>
-      <c r="I33">
-        <v>1.4999999999999999E-2</v>
+      <c r="H33">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I33" s="1">
+        <v>26834</v>
       </c>
       <c r="J33" s="1">
-        <v>26834</v>
+        <f t="shared" si="3"/>
+        <v>29011</v>
       </c>
       <c r="K33" s="1">
-        <v>26835</v>
-      </c>
-      <c r="L33" s="1">
         <v>2464</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1794,33 +1758,31 @@
       <c r="D34" t="b">
         <v>1</v>
       </c>
-      <c r="E34" t="s">
-        <v>23</v>
+      <c r="E34" s="1">
+        <v>20500</v>
       </c>
       <c r="F34" s="1">
-        <v>20500</v>
-      </c>
-      <c r="G34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>22163</v>
       </c>
-      <c r="H34" s="3">
+      <c r="G34" s="3">
         <v>0.2</v>
       </c>
-      <c r="I34">
-        <v>1.4999999999999999E-2</v>
+      <c r="H34">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I34" s="1">
+        <v>31729</v>
       </c>
       <c r="J34" s="1">
-        <v>31729</v>
+        <f t="shared" si="3"/>
+        <v>34303</v>
       </c>
       <c r="K34" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L34" s="1">
         <v>2464</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -1833,33 +1795,31 @@
       <c r="D35" t="b">
         <v>0</v>
       </c>
-      <c r="E35" t="s">
-        <v>23</v>
+      <c r="E35" s="1">
+        <v>19252</v>
       </c>
       <c r="F35" s="1">
-        <v>19252</v>
-      </c>
-      <c r="G35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>20814</v>
       </c>
-      <c r="H35" s="3">
+      <c r="G35" s="3">
         <v>0.2</v>
       </c>
-      <c r="I35">
-        <v>1.4999999999999999E-2</v>
+      <c r="H35">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I35" s="1">
+        <v>31729</v>
       </c>
       <c r="J35" s="1">
-        <v>31729</v>
+        <f t="shared" si="3"/>
+        <v>34303</v>
       </c>
       <c r="K35" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L35" s="1">
         <v>2464</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -1872,33 +1832,31 @@
       <c r="D36" t="b">
         <v>0</v>
       </c>
-      <c r="E36" t="s">
-        <v>23</v>
+      <c r="E36" s="1">
+        <v>15529</v>
       </c>
       <c r="F36" s="1">
-        <v>15529</v>
-      </c>
-      <c r="G36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v>16789</v>
       </c>
-      <c r="H36" s="3">
+      <c r="G36" s="3">
         <v>0.2</v>
       </c>
-      <c r="I36">
-        <v>1.4999999999999999E-2</v>
+      <c r="H36">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I36" s="1">
+        <v>26205</v>
       </c>
       <c r="J36" s="1">
-        <v>26205</v>
+        <f t="shared" si="3"/>
+        <v>28331</v>
       </c>
       <c r="K36" s="1">
-        <v>26206</v>
-      </c>
-      <c r="L36" s="1">
         <v>2406</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -1911,33 +1869,31 @@
       <c r="D37" t="b">
         <v>1</v>
       </c>
-      <c r="E37" t="s">
-        <v>23</v>
+      <c r="E37" s="1">
+        <v>20500</v>
       </c>
       <c r="F37" s="1">
-        <v>20500</v>
-      </c>
-      <c r="G37" s="1">
-        <f>ROUND((F37 +1)*H37/(H37-I37), 0)</f>
+        <f t="shared" si="0"/>
         <v>22163</v>
       </c>
-      <c r="H37" s="3">
+      <c r="G37" s="3">
         <v>0.2</v>
       </c>
-      <c r="I37">
-        <v>1.4999999999999999E-2</v>
+      <c r="H37">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I37" s="1">
+        <v>31729</v>
       </c>
       <c r="J37" s="1">
-        <v>31729</v>
+        <f t="shared" si="3"/>
+        <v>34303</v>
       </c>
       <c r="K37" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L37" s="1">
         <v>2406</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -1950,348 +1906,330 @@
       <c r="D38" t="b">
         <v>0</v>
       </c>
-      <c r="E38" t="s">
-        <v>23</v>
+      <c r="E38" s="1">
+        <v>18141</v>
       </c>
       <c r="F38" s="1">
-        <v>18141</v>
-      </c>
-      <c r="G38" s="1">
-        <f t="shared" ref="G38:G54" si="4">ROUND((F38 +1)*H38/(H38-I38), 0)</f>
+        <f t="shared" si="0"/>
         <v>19613</v>
       </c>
-      <c r="H38" s="3">
+      <c r="G38" s="3">
         <v>0.2</v>
       </c>
-      <c r="I38">
-        <v>1.4999999999999999E-2</v>
+      <c r="H38">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I38" s="1">
+        <v>31729</v>
       </c>
       <c r="J38" s="1">
+        <f t="shared" si="3"/>
+        <v>34303</v>
+      </c>
+      <c r="K38" s="1">
+        <v>2406</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" t="b">
+        <v>0</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>15062</v>
+      </c>
+      <c r="F39" s="1">
+        <f t="shared" si="0"/>
+        <v>16284</v>
+      </c>
+      <c r="G39" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H39">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I39" s="1">
+        <v>25417</v>
+      </c>
+      <c r="J39" s="1">
+        <f t="shared" si="3"/>
+        <v>27479</v>
+      </c>
+      <c r="K39" s="1">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E40" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F40" s="1">
+        <f t="shared" ref="F38:F54" si="4">ROUND((E40 +1)*G40/(G40-H40), 0)</f>
+        <v>21623</v>
+      </c>
+      <c r="G40" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H40">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I40" s="1">
         <v>31729</v>
       </c>
-      <c r="K38" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L38" s="1">
-        <v>2406</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="J40" s="1">
+        <f t="shared" si="3"/>
+        <v>34303</v>
+      </c>
+      <c r="K40" s="1">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>17164</v>
+      </c>
+      <c r="F41" s="1">
+        <f t="shared" si="4"/>
+        <v>18557</v>
+      </c>
+      <c r="G41" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H41">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I41" s="1">
+        <v>31729</v>
+      </c>
+      <c r="J41" s="1">
+        <f t="shared" si="3"/>
+        <v>34303</v>
+      </c>
+      <c r="K41" s="1">
+        <v>2334</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>32</v>
       </c>
-      <c r="B39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" t="b">
-        <v>0</v>
-      </c>
-      <c r="E39" t="s">
-        <v>23</v>
-      </c>
-      <c r="F39" s="1">
-        <v>15062</v>
-      </c>
-      <c r="G39" s="1">
+      <c r="B42" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="1">
+        <v>14539</v>
+      </c>
+      <c r="F42" s="1">
         <f t="shared" si="4"/>
-        <v>16284</v>
-      </c>
-      <c r="H39" s="3">
+        <v>15719</v>
+      </c>
+      <c r="G42" s="3">
         <v>0.2</v>
       </c>
-      <c r="I39">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J39" s="1">
-        <v>25417</v>
-      </c>
-      <c r="K39" s="1">
-        <v>25418</v>
-      </c>
-      <c r="L39" s="1">
-        <v>2334</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="H42">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I42" s="1">
+        <v>24534</v>
+      </c>
+      <c r="J42" s="1">
+        <f t="shared" si="3"/>
+        <v>26524</v>
+      </c>
+      <c r="K42" s="1">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>32</v>
       </c>
-      <c r="B40" t="b">
-        <v>1</v>
-      </c>
-      <c r="C40" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>23</v>
-      </c>
-      <c r="F40" s="1">
+      <c r="B43" t="b">
+        <v>1</v>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" t="b">
+        <v>1</v>
+      </c>
+      <c r="E43" s="1">
         <v>20000</v>
       </c>
-      <c r="G40" s="1">
+      <c r="F43" s="1">
         <f t="shared" si="4"/>
         <v>21623</v>
       </c>
-      <c r="H40" s="3">
+      <c r="G43" s="3">
         <v>0.2</v>
       </c>
-      <c r="I40">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J40" s="1">
+      <c r="H43">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I43" s="1">
         <v>31729</v>
       </c>
-      <c r="K40" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L40" s="1">
-        <v>2334</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="J43" s="1">
+        <f t="shared" si="3"/>
+        <v>34303</v>
+      </c>
+      <c r="K43" s="1">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>32</v>
       </c>
-      <c r="B41" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" t="b">
-        <v>1</v>
-      </c>
-      <c r="D41" t="b">
-        <v>0</v>
-      </c>
-      <c r="E41" t="s">
-        <v>23</v>
-      </c>
-      <c r="F41" s="1">
-        <v>17164</v>
-      </c>
-      <c r="G41" s="1">
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>16570</v>
+      </c>
+      <c r="F44" s="1">
         <f t="shared" si="4"/>
-        <v>18557</v>
-      </c>
-      <c r="H41" s="3">
+        <v>17915</v>
+      </c>
+      <c r="G44" s="3">
         <v>0.2</v>
       </c>
-      <c r="I41">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J41" s="1">
+      <c r="H44">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I44" s="1">
         <v>31729</v>
       </c>
-      <c r="K41" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L41" s="1">
-        <v>2334</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="J44" s="1">
+        <f t="shared" si="3"/>
+        <v>34303</v>
+      </c>
+      <c r="K44" s="1">
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>33</v>
       </c>
-      <c r="B42" t="b">
-        <v>0</v>
-      </c>
-      <c r="C42" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>23</v>
-      </c>
-      <c r="F42" s="1">
-        <v>14539</v>
-      </c>
-      <c r="G42" s="1">
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" t="b">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>13807</v>
+      </c>
+      <c r="F45" s="1">
         <f t="shared" si="4"/>
-        <v>15719</v>
-      </c>
-      <c r="H42" s="3">
+        <v>14928</v>
+      </c>
+      <c r="G45" s="3">
         <v>0.2</v>
       </c>
-      <c r="I42">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J42" s="1">
-        <v>24534</v>
-      </c>
-      <c r="K42" s="1">
-        <v>24535</v>
-      </c>
-      <c r="L42" s="1">
-        <v>2253</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="H45">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I45" s="1">
+        <v>23300</v>
+      </c>
+      <c r="J45" s="1">
+        <f t="shared" si="3"/>
+        <v>25190</v>
+      </c>
+      <c r="K45" s="1">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>33</v>
       </c>
-      <c r="B43" t="b">
-        <v>1</v>
-      </c>
-      <c r="C43" t="b">
-        <v>0</v>
-      </c>
-      <c r="D43" t="b">
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>23</v>
-      </c>
-      <c r="F43" s="1">
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1">
         <v>20000</v>
       </c>
-      <c r="G43" s="1">
+      <c r="F46" s="1">
         <f t="shared" si="4"/>
         <v>21623</v>
       </c>
-      <c r="H43" s="3">
+      <c r="G46" s="3">
         <v>0.2</v>
       </c>
-      <c r="I43">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J43" s="1">
+      <c r="H46">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I46" s="1">
         <v>31729</v>
       </c>
-      <c r="K43" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L43" s="1">
-        <v>2253</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="J46" s="1">
+        <f t="shared" si="3"/>
+        <v>34303</v>
+      </c>
+      <c r="K46" s="1">
+        <v>2140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>33</v>
       </c>
-      <c r="B44" t="b">
-        <v>0</v>
-      </c>
-      <c r="C44" t="b">
-        <v>1</v>
-      </c>
-      <c r="D44" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
-        <v>23</v>
-      </c>
-      <c r="F44" s="1">
-        <v>16570</v>
-      </c>
-      <c r="G44" s="1">
-        <f t="shared" si="4"/>
-        <v>17915</v>
-      </c>
-      <c r="H44" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I44">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J44" s="1">
-        <v>31729</v>
-      </c>
-      <c r="K44" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L44" s="1">
-        <v>2253</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45" t="b">
-        <v>0</v>
-      </c>
-      <c r="D45" t="b">
-        <v>0</v>
-      </c>
-      <c r="E45" t="s">
-        <v>23</v>
-      </c>
-      <c r="F45" s="1">
-        <v>13807</v>
-      </c>
-      <c r="G45" s="1">
-        <f t="shared" si="4"/>
-        <v>14928</v>
-      </c>
-      <c r="H45" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I45">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J45" s="1">
-        <v>23300</v>
-      </c>
-      <c r="K45" s="1">
-        <v>23301</v>
-      </c>
-      <c r="L45" s="1">
-        <v>2140</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" t="b">
-        <v>1</v>
-      </c>
-      <c r="C46" t="b">
-        <v>0</v>
-      </c>
-      <c r="D46" t="b">
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>23</v>
-      </c>
-      <c r="F46" s="1">
-        <v>20000</v>
-      </c>
-      <c r="G46" s="1">
-        <f t="shared" si="4"/>
-        <v>21623</v>
-      </c>
-      <c r="H46" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="I46">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="J46" s="1">
-        <v>31729</v>
-      </c>
-      <c r="K46" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L46" s="1">
-        <v>2140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>34</v>
-      </c>
       <c r="B47" t="b">
         <v>0</v>
       </c>
@@ -2301,35 +2239,33 @@
       <c r="D47" t="b">
         <v>0</v>
       </c>
-      <c r="E47" t="s">
-        <v>23</v>
+      <c r="E47" s="1">
+        <v>15970</v>
       </c>
       <c r="F47" s="1">
-        <v>15970</v>
-      </c>
-      <c r="G47" s="1">
         <f t="shared" si="4"/>
         <v>17266</v>
       </c>
-      <c r="H47" s="3">
+      <c r="G47" s="3">
         <v>0.2</v>
       </c>
-      <c r="I47">
-        <v>1.4999999999999999E-2</v>
+      <c r="H47">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I47" s="1">
+        <v>31729</v>
       </c>
       <c r="J47" s="1">
-        <v>31729</v>
+        <f t="shared" si="3"/>
+        <v>34303</v>
       </c>
       <c r="K47" s="1">
-        <v>31730</v>
-      </c>
-      <c r="L47" s="1">
         <v>2140</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B48" t="b">
         <v>0</v>
@@ -2340,26 +2276,23 @@
       <c r="D48" t="b">
         <v>0</v>
       </c>
-      <c r="E48" t="s">
-        <v>23</v>
+      <c r="E48" s="1">
+        <v>13351</v>
       </c>
       <c r="F48" s="1">
-        <v>13351</v>
-      </c>
-      <c r="G48" s="1">
         <f t="shared" si="4"/>
         <v>14435</v>
       </c>
-      <c r="H48" s="3">
+      <c r="G48" s="3">
         <v>0.2</v>
       </c>
-      <c r="I48">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H48">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B49" t="b">
         <v>0</v>
@@ -2370,26 +2303,23 @@
       <c r="D49" t="b">
         <v>0</v>
       </c>
-      <c r="E49" t="s">
-        <v>36</v>
+      <c r="E49" s="1">
+        <v>22866</v>
       </c>
       <c r="F49" s="1">
-        <v>22866</v>
-      </c>
-      <c r="G49" s="1">
         <f t="shared" si="4"/>
         <v>24721</v>
       </c>
-      <c r="H49" s="3">
+      <c r="G49" s="3">
         <v>0.2</v>
       </c>
-      <c r="I49">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H49">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B50" t="b">
         <v>0</v>
@@ -2400,26 +2330,23 @@
       <c r="D50" t="b">
         <v>0</v>
       </c>
-      <c r="E50" t="s">
-        <v>37</v>
+      <c r="E50" s="1">
+        <v>24966</v>
       </c>
       <c r="F50" s="1">
-        <v>24966</v>
-      </c>
-      <c r="G50" s="1">
         <f t="shared" si="4"/>
         <v>26991</v>
       </c>
-      <c r="H50" s="3">
+      <c r="G50" s="3">
         <v>0.2</v>
       </c>
-      <c r="I50">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B51" t="b">
         <v>0</v>
@@ -2430,26 +2357,23 @@
       <c r="D51" t="b">
         <v>0</v>
       </c>
-      <c r="E51" t="s">
-        <v>38</v>
+      <c r="E51" s="1">
+        <v>24966</v>
       </c>
       <c r="F51" s="1">
-        <v>24966</v>
-      </c>
-      <c r="G51" s="1">
         <f t="shared" si="4"/>
         <v>26991</v>
       </c>
-      <c r="H51" s="3">
+      <c r="G51" s="3">
         <v>0.2</v>
       </c>
-      <c r="I51">
-        <v>1.4999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H51">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B52" t="b">
         <v>0</v>
@@ -2460,14 +2384,14 @@
       <c r="D52" t="b">
         <v>0</v>
       </c>
-      <c r="G52" s="1" t="e">
+      <c r="F52" s="1" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B53" t="b">
         <v>1</v>
@@ -2478,14 +2402,14 @@
       <c r="D53" t="b">
         <v>1</v>
       </c>
-      <c r="G53" s="1" t="e">
+      <c r="F53" s="1" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B54" t="b">
         <v>0</v>
@@ -2496,13 +2420,13 @@
       <c r="D54" t="b">
         <v>0</v>
       </c>
-      <c r="G54" s="1" t="e">
+      <c r="F54" s="1" t="e">
         <f t="shared" si="4"/>
         <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L32">
+  <sortState ref="A2:K32">
     <sortCondition descending="1" ref="A2:A32"/>
     <sortCondition ref="D2:D32"/>
     <sortCondition ref="B2:B32"/>
@@ -2541,19 +2465,19 @@
         <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" t="s">
         <v>21</v>
@@ -2573,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2">
         <v>33693</v>
@@ -2602,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3">
         <v>46000</v>
@@ -2631,7 +2555,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4">
         <v>34367</v>
@@ -2660,7 +2584,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5">
         <v>46000</v>
@@ -2689,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>35261</v>
@@ -2718,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F7">
         <v>46000</v>
@@ -2747,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8">
         <v>36001</v>
@@ -2776,7 +2700,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9">
         <v>46966</v>
@@ -2799,13 +2723,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10">
         <v>36001</v>
@@ -2828,13 +2752,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11">
         <v>46966</v>
@@ -2865,27 +2789,38 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="71.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reunite xlsx and sysdata.rda
</commit_message>
<xml_diff>
--- a/data-raw/medicare-tables.xlsx
+++ b/data-raw/medicare-tables.xlsx
@@ -652,11 +652,11 @@
         <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>20896</v>
+        <v>21335</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>26121</v>
+        <v>26670</v>
       </c>
       <c r="G4" s="3">
         <v>0.1</v>
@@ -691,11 +691,11 @@
         <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>33044</v>
+        <v>33738</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>41306</v>
+        <v>42174</v>
       </c>
       <c r="G5" s="3">
         <v>0.1</v>
@@ -729,11 +729,11 @@
         <v>0</v>
       </c>
       <c r="E6" s="1">
-        <v>20542</v>
+        <v>20896</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>25679</v>
+        <v>26121</v>
       </c>
       <c r="G6" s="3">
         <v>0.1</v>
@@ -742,14 +742,14 @@
         <v>0.02</v>
       </c>
       <c r="I6" s="1">
-        <v>34367</v>
+        <v>35261</v>
       </c>
       <c r="J6" s="1">
         <f t="shared" si="3"/>
-        <v>42960</v>
+        <v>44078</v>
       </c>
       <c r="K6" s="1">
-        <v>3156</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -768,11 +768,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
-        <v>32279</v>
+        <v>33044</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>40350</v>
+        <v>41306</v>
       </c>
       <c r="G7" s="3">
         <v>0.1</v>
@@ -788,7 +788,7 @@
         <v>57501</v>
       </c>
       <c r="K7" s="1">
-        <v>3156</v>
+        <v>3238</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -1984,7 +1984,7 @@
         <v>20000</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" ref="F38:F54" si="4">ROUND((E40 +1)*G40/(G40-H40), 0)</f>
+        <f t="shared" ref="F40:F54" si="4">ROUND((E40 +1)*G40/(G40-H40), 0)</f>
         <v>21623</v>
       </c>
       <c r="G40" s="3">

</xml_diff>

<commit_message>
Never-legislated Medicare levy change reverted
</commit_message>
<xml_diff>
--- a/data-raw/medicare-tables.xlsx
+++ b/data-raw/medicare-tables.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hughp\Documents\grattan\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D193289-F989-4A71-9529-3A73DD44FDEC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="7485"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15315" windowHeight="7485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indiv" sheetId="1" r:id="rId1"/>
     <sheet name="families" sheetId="3" r:id="rId2"/>
     <sheet name="SourceURL" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -151,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -524,12 +525,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,13 +599,13 @@
       </c>
       <c r="F2" s="1">
         <f t="shared" ref="F2:F5" si="0">ROUND((E2 +1)*G2/(G2-H2), 0)</f>
-        <v>28875</v>
+        <v>27070</v>
       </c>
       <c r="G2" s="4">
         <v>0.1</v>
       </c>
       <c r="H2" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="I2" s="1">
         <v>36001</v>
@@ -634,13 +635,13 @@
       </c>
       <c r="F3" s="1">
         <f t="shared" si="0"/>
-        <v>45660</v>
+        <v>42806</v>
       </c>
       <c r="G3" s="4">
         <v>0.1</v>
       </c>
       <c r="H3" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="I3" s="1">
         <v>46966</v>
@@ -2679,7 +2680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3031,7 +3032,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
correct medicare levy thresholds
</commit_message>
<xml_diff>
--- a/data-raw/medicare-tables.xlsx
+++ b/data-raw/medicare-tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mcowgill/Dropbox (Personal)/R/packages/hughparsonage/grattan/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F853D338-5C4C-2C4E-9638-2D5ECD4268AF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223544E0-4F14-3443-BE42-346174AD2FB2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="2660" windowWidth="19000" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2360" yWindow="980" windowWidth="19000" windowHeight="13300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="indiv" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
   <si>
     <t>fy_year</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>2019-20: p19 in BP2</t>
-  </si>
-  <si>
-    <t>2020-21</t>
   </si>
   <si>
     <t>Relevant section of Medicare Levy Act for family thresholds:</t>
@@ -174,8 +171,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -218,7 +214,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -233,7 +229,6 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -549,11 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:K60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -568,7 +563,7 @@
     <col min="11" max="11" width="25.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -603,9 +598,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -620,7 +615,7 @@
         <v>22398</v>
       </c>
       <c r="F2" s="1">
-        <f t="shared" ref="F2:F7" si="0">ROUND((E2 +1)*G2/(G2-H2), 0)</f>
+        <f t="shared" ref="F2:F3" si="0">ROUND((E2 +1)*G2/(G2-H2), 0)</f>
         <v>27999</v>
       </c>
       <c r="G2" s="4">
@@ -633,17 +628,16 @@
         <v>37794</v>
       </c>
       <c r="J2" s="1">
-        <f t="shared" ref="J2:J4" si="1">ROUND((I2 +1)*G2/(G2-H2), 0)</f>
+        <f t="shared" ref="J2" si="1">ROUND((I2 +1)*G2/(G2-H2), 0)</f>
         <v>47244</v>
       </c>
       <c r="K2" s="1">
         <v>3471</v>
       </c>
-      <c r="L2" s="6"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -678,11 +672,12 @@
         <v>3471</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="b">
+        <f>D4</f>
         <v>0</v>
       </c>
       <c r="C4" t="b">
@@ -695,7 +690,7 @@
         <v>21980</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F4:F5" si="2">ROUND((E4 +1)*G4/(G4-H4), 0)</f>
         <v>27476</v>
       </c>
       <c r="G4" s="4">
@@ -714,14 +709,16 @@
         <v>3406</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" t="b">
+        <f t="shared" ref="B5" si="3">D5</f>
         <v>1</v>
       </c>
       <c r="C5" t="b">
+        <f t="shared" ref="C5" si="4">NOT(D5)</f>
         <v>0</v>
       </c>
       <c r="D5" t="b">
@@ -731,7 +728,7 @@
         <v>34758</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>43449</v>
       </c>
       <c r="G5" s="4">
@@ -751,9 +748,9 @@
         <v>3406</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="b">
         <f>D6</f>
@@ -769,7 +766,7 @@
         <v>21980</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F6:F7" si="5">ROUND((E6 +1)*G6/(G6-H6), 0)</f>
         <v>27476</v>
       </c>
       <c r="G6" s="4">
@@ -788,16 +785,16 @@
         <v>3406</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" t="b">
-        <f t="shared" ref="B7" si="2">D7</f>
+        <f t="shared" ref="B7" si="6">D7</f>
         <v>1</v>
       </c>
       <c r="C7" t="b">
-        <f t="shared" ref="C7" si="3">NOT(D7)</f>
+        <f t="shared" ref="C7" si="7">NOT(D7)</f>
         <v>0</v>
       </c>
       <c r="D7" t="b">
@@ -807,7 +804,7 @@
         <v>34758</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>43449</v>
       </c>
       <c r="G7" s="4">
@@ -827,9 +824,9 @@
         <v>3406</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B8" t="b">
         <f>D8</f>
@@ -842,73 +839,73 @@
         <v>0</v>
       </c>
       <c r="E8" s="1">
-        <v>21980</v>
+        <v>21665</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" ref="F8:F9" si="4">ROUND((E8 +1)*G8/(G8-H8), 0)</f>
-        <v>27476</v>
-      </c>
-      <c r="G8" s="4">
+        <f t="shared" ref="F8:F45" si="8">ROUND((E8 +1)*G8/(G8-H8), 0)</f>
+        <v>27083</v>
+      </c>
+      <c r="G8" s="5">
         <v>0.1</v>
       </c>
       <c r="H8" s="4">
         <v>0.02</v>
       </c>
       <c r="I8" s="1">
-        <v>37089</v>
+        <v>36541</v>
       </c>
       <c r="J8" s="1">
         <v>45676</v>
       </c>
       <c r="K8" s="1">
-        <v>3406</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="B9" t="b">
-        <f t="shared" ref="B9" si="5">D9</f>
+        <f t="shared" ref="B9:B17" si="9">D9</f>
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <f t="shared" ref="C9" si="6">NOT(D9)</f>
+        <f t="shared" ref="C9:C17" si="10">NOT(D9)</f>
         <v>0</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>34758</v>
+        <v>34244</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="4"/>
-        <v>43449</v>
-      </c>
-      <c r="G9" s="4">
+        <f t="shared" si="8"/>
+        <v>42806</v>
+      </c>
+      <c r="G9" s="5">
         <v>0.1</v>
       </c>
       <c r="H9" s="4">
         <v>0.02</v>
       </c>
       <c r="I9" s="1">
-        <v>48385</v>
+        <v>47670</v>
       </c>
       <c r="J9" s="1">
         <f>ROUND((I9 +1)*G9/(G9-H9), 0)</f>
-        <v>60483</v>
+        <v>59589</v>
       </c>
       <c r="K9" s="1">
-        <v>3406</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B10" t="b">
-        <f>D10</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C10" t="b">
@@ -918,11 +915,11 @@
         <v>0</v>
       </c>
       <c r="E10" s="1">
-        <v>21665</v>
+        <v>21335</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" ref="F10:F47" si="7">ROUND((E10 +1)*G10/(G10-H10), 0)</f>
-        <v>27083</v>
+        <f t="shared" si="8"/>
+        <v>26670</v>
       </c>
       <c r="G10" s="5">
         <v>0.1</v>
@@ -931,36 +928,37 @@
         <v>0.02</v>
       </c>
       <c r="I10" s="1">
-        <v>36541</v>
+        <v>35261</v>
       </c>
       <c r="J10" s="1">
-        <v>45676</v>
+        <f t="shared" ref="J10:J53" si="11">ROUND((I10 +1)*G10/(G10-H10), 0)</f>
+        <v>44078</v>
       </c>
       <c r="K10" s="1">
-        <v>3356</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B11" t="b">
-        <f t="shared" ref="B11:B19" si="8">D11</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="C11" t="b">
-        <f t="shared" ref="C11:C19" si="9">NOT(D11)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="1">
-        <v>34244</v>
+        <v>33738</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="7"/>
-        <v>42806</v>
+        <f t="shared" si="8"/>
+        <v>42174</v>
       </c>
       <c r="G11" s="5">
         <v>0.1</v>
@@ -969,22 +967,22 @@
         <v>0.02</v>
       </c>
       <c r="I11" s="1">
-        <v>47670</v>
+        <v>46966</v>
       </c>
       <c r="J11" s="1">
-        <f>ROUND((I11 +1)*G11/(G11-H11), 0)</f>
-        <v>59589</v>
+        <f t="shared" si="11"/>
+        <v>58709</v>
       </c>
       <c r="K11" s="1">
-        <v>3356</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C12" t="b">
@@ -994,11 +992,11 @@
         <v>0</v>
       </c>
       <c r="E12" s="1">
-        <v>21335</v>
+        <v>20896</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="7"/>
-        <v>26670</v>
+        <f t="shared" si="8"/>
+        <v>26121</v>
       </c>
       <c r="G12" s="5">
         <v>0.1</v>
@@ -1010,34 +1008,34 @@
         <v>35261</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" ref="J12:J55" si="10">ROUND((I12 +1)*G12/(G12-H12), 0)</f>
+        <f t="shared" si="11"/>
         <v>44078</v>
       </c>
       <c r="K12" s="1">
         <v>3238</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="C13" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>33738</v>
+        <v>33044</v>
       </c>
       <c r="F13" s="1">
-        <f t="shared" si="7"/>
-        <v>42174</v>
+        <f t="shared" si="8"/>
+        <v>41306</v>
       </c>
       <c r="G13" s="5">
         <v>0.1</v>
@@ -1046,22 +1044,22 @@
         <v>0.02</v>
       </c>
       <c r="I13" s="1">
-        <v>46966</v>
+        <v>46000</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="10"/>
-        <v>58709</v>
+        <f t="shared" si="11"/>
+        <v>57501</v>
       </c>
       <c r="K13" s="1">
         <v>3238</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B14" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C14" t="b">
@@ -1071,74 +1069,74 @@
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>20896</v>
+        <v>20542</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="7"/>
-        <v>26121</v>
+        <f t="shared" si="8"/>
+        <v>24168</v>
       </c>
       <c r="G14" s="5">
         <v>0.1</v>
       </c>
-      <c r="H14" s="4">
-        <v>0.02</v>
+      <c r="H14" s="3">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="I14" s="1">
-        <v>35261</v>
+        <v>34367</v>
       </c>
       <c r="J14" s="1">
+        <f t="shared" si="11"/>
+        <v>40433</v>
+      </c>
+      <c r="K14" s="1">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="C15" t="b">
         <f t="shared" si="10"/>
-        <v>44078</v>
-      </c>
-      <c r="K14" s="1">
-        <v>3238</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="b">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="C15" t="b">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="D15" t="b">
         <v>1</v>
       </c>
       <c r="E15" s="1">
-        <v>33044</v>
+        <v>32279</v>
       </c>
       <c r="F15" s="1">
-        <f t="shared" si="7"/>
-        <v>41306</v>
+        <f t="shared" si="8"/>
+        <v>37976</v>
       </c>
       <c r="G15" s="5">
         <v>0.1</v>
       </c>
-      <c r="H15" s="4">
-        <v>0.02</v>
+      <c r="H15" s="3">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="I15" s="1">
         <v>46000</v>
       </c>
       <c r="J15" s="1">
-        <f t="shared" si="10"/>
-        <v>57501</v>
+        <f t="shared" si="11"/>
+        <v>54119</v>
       </c>
       <c r="K15" s="1">
-        <v>3238</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>3156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B16" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="C16" t="b">
@@ -1151,7 +1149,7 @@
         <v>20542</v>
       </c>
       <c r="F16" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>24168</v>
       </c>
       <c r="G16" s="5">
@@ -1161,26 +1159,26 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>34367</v>
+        <v>33693</v>
       </c>
       <c r="J16" s="1">
-        <f t="shared" si="10"/>
-        <v>40433</v>
+        <f t="shared" si="11"/>
+        <v>39640</v>
       </c>
       <c r="K16" s="1">
-        <v>3156</v>
+        <v>3094</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B17" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="C17" t="b">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="D17" t="b">
@@ -1190,7 +1188,7 @@
         <v>32279</v>
       </c>
       <c r="F17" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>37976</v>
       </c>
       <c r="G17" s="5">
@@ -1203,19 +1201,18 @@
         <v>46000</v>
       </c>
       <c r="J17" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>54119</v>
       </c>
       <c r="K17" s="1">
-        <v>3156</v>
+        <v>3094</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B18" t="b">
-        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="C18" t="b">
@@ -1225,11 +1222,11 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <v>20542</v>
+        <v>19404</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="7"/>
-        <v>24168</v>
+        <f t="shared" si="8"/>
+        <v>22829</v>
       </c>
       <c r="G18" s="5">
         <v>0.1</v>
@@ -1238,37 +1235,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I18" s="1">
-        <v>33693</v>
+        <v>32743</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="10"/>
-        <v>39640</v>
+        <f t="shared" si="11"/>
+        <v>38522</v>
       </c>
       <c r="K18" s="1">
-        <v>3094</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" t="b">
-        <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="b">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1">
-        <v>32279</v>
+        <v>30452</v>
       </c>
       <c r="F19" s="1">
-        <f t="shared" si="7"/>
-        <v>37976</v>
+        <f t="shared" si="8"/>
+        <v>35827</v>
       </c>
       <c r="G19" s="5">
         <v>0.1</v>
@@ -1277,14 +1272,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I19" s="1">
-        <v>46000</v>
+        <v>32743</v>
       </c>
       <c r="J19" s="1">
-        <f t="shared" si="10"/>
-        <v>54119</v>
+        <f t="shared" si="11"/>
+        <v>38522</v>
       </c>
       <c r="K19" s="1">
-        <v>3094</v>
+        <v>3007</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1292,20 +1287,20 @@
         <v>4</v>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
       </c>
       <c r="D20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>19404</v>
+        <v>30685</v>
       </c>
       <c r="F20" s="1">
-        <f t="shared" si="7"/>
-        <v>22829</v>
+        <f t="shared" si="8"/>
+        <v>36101</v>
       </c>
       <c r="G20" s="5">
         <v>0.1</v>
@@ -1314,11 +1309,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I20" s="1">
-        <v>32743</v>
+        <v>44500</v>
       </c>
       <c r="J20" s="1">
-        <f t="shared" si="10"/>
-        <v>38522</v>
+        <f t="shared" si="11"/>
+        <v>52354</v>
       </c>
       <c r="K20" s="1">
         <v>3007</v>
@@ -1326,23 +1321,23 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
       </c>
       <c r="C21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
       </c>
       <c r="E21" s="1">
-        <v>30452</v>
+        <v>18839</v>
       </c>
       <c r="F21" s="1">
-        <f t="shared" si="7"/>
-        <v>35827</v>
+        <f t="shared" si="8"/>
+        <v>22165</v>
       </c>
       <c r="G21" s="5">
         <v>0.1</v>
@@ -1351,35 +1346,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I21" s="1">
-        <v>32743</v>
+        <v>31789</v>
       </c>
       <c r="J21" s="1">
-        <f t="shared" si="10"/>
-        <v>38522</v>
+        <f t="shared" si="11"/>
+        <v>37400</v>
       </c>
       <c r="K21" s="1">
-        <v>3007</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22" s="1">
-        <v>30685</v>
+        <v>30439</v>
       </c>
       <c r="F22" s="1">
-        <f t="shared" si="7"/>
-        <v>36101</v>
+        <f t="shared" si="8"/>
+        <v>35812</v>
       </c>
       <c r="G22" s="5">
         <v>0.1</v>
@@ -1387,15 +1382,8 @@
       <c r="H22" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I22" s="1">
-        <v>44500</v>
-      </c>
-      <c r="J22" s="1">
-        <f t="shared" si="10"/>
-        <v>52354</v>
-      </c>
       <c r="K22" s="1">
-        <v>3007</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
@@ -1403,20 +1391,20 @@
         <v>8</v>
       </c>
       <c r="B23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
       </c>
       <c r="D23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>18839</v>
+        <v>30685</v>
       </c>
       <c r="F23" s="1">
-        <f t="shared" si="7"/>
-        <v>22165</v>
+        <f t="shared" si="8"/>
+        <v>36101</v>
       </c>
       <c r="G23" s="5">
         <v>0.1</v>
@@ -1425,11 +1413,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I23" s="1">
-        <v>31789</v>
+        <v>44500</v>
       </c>
       <c r="J23" s="1">
-        <f t="shared" si="10"/>
-        <v>37400</v>
+        <f t="shared" si="11"/>
+        <v>52354</v>
       </c>
       <c r="K23" s="1">
         <v>2919</v>
@@ -1437,23 +1425,23 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" t="b">
         <v>0</v>
       </c>
       <c r="C24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D24" t="b">
         <v>0</v>
       </c>
       <c r="E24" s="1">
-        <v>30439</v>
+        <v>18488</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="7"/>
-        <v>35812</v>
+        <f t="shared" si="8"/>
+        <v>21752</v>
       </c>
       <c r="G24" s="5">
         <v>0.1</v>
@@ -1461,29 +1449,36 @@
       <c r="H24" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="I24" s="1">
+        <v>31196</v>
+      </c>
+      <c r="J24" s="1">
+        <f t="shared" si="11"/>
+        <v>36702</v>
+      </c>
       <c r="K24" s="1">
-        <v>2919</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25" s="1">
-        <v>30685</v>
+        <v>27697</v>
       </c>
       <c r="F25" s="1">
-        <f t="shared" si="7"/>
-        <v>36101</v>
+        <f t="shared" si="8"/>
+        <v>32586</v>
       </c>
       <c r="G25" s="5">
         <v>0.1</v>
@@ -1491,15 +1486,8 @@
       <c r="H25" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I25" s="1">
-        <v>44500</v>
-      </c>
-      <c r="J25" s="1">
-        <f t="shared" si="10"/>
-        <v>52354</v>
-      </c>
       <c r="K25" s="1">
-        <v>2919</v>
+        <v>2865</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
@@ -1507,20 +1495,20 @@
         <v>9</v>
       </c>
       <c r="B26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
       </c>
       <c r="D26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>18488</v>
+        <v>29867</v>
       </c>
       <c r="F26" s="1">
-        <f t="shared" si="7"/>
-        <v>21752</v>
+        <f t="shared" si="8"/>
+        <v>35139</v>
       </c>
       <c r="G26" s="5">
         <v>0.1</v>
@@ -1529,11 +1517,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I26" s="1">
-        <v>31196</v>
+        <v>43500</v>
       </c>
       <c r="J26" s="1">
-        <f t="shared" si="10"/>
-        <v>36702</v>
+        <f t="shared" si="11"/>
+        <v>51178</v>
       </c>
       <c r="K26" s="1">
         <v>2865</v>
@@ -1541,23 +1529,23 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B27" t="b">
         <v>0</v>
       </c>
       <c r="C27" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D27" t="b">
         <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>27697</v>
+        <v>17794</v>
       </c>
       <c r="F27" s="1">
-        <f t="shared" si="7"/>
-        <v>32586</v>
+        <f t="shared" si="8"/>
+        <v>20935</v>
       </c>
       <c r="G27" s="5">
         <v>0.1</v>
@@ -1565,29 +1553,36 @@
       <c r="H27" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
+      <c r="I27" s="1">
+        <v>30025</v>
+      </c>
+      <c r="J27" s="1">
+        <f t="shared" si="11"/>
+        <v>35325</v>
+      </c>
       <c r="K27" s="1">
-        <v>2865</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C28" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28" s="1">
-        <v>29867</v>
+        <v>25299</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="7"/>
-        <v>35139</v>
+        <f t="shared" si="8"/>
+        <v>29765</v>
       </c>
       <c r="G28" s="5">
         <v>0.1</v>
@@ -1596,14 +1591,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I28" s="1">
-        <v>43500</v>
+        <v>42000</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="10"/>
-        <v>51178</v>
+        <f t="shared" si="11"/>
+        <v>49413</v>
       </c>
       <c r="K28" s="1">
-        <v>2865</v>
+        <v>2757</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1611,20 +1606,20 @@
         <v>10</v>
       </c>
       <c r="B29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
       <c r="D29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="1">
-        <v>17794</v>
+        <v>28867</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="7"/>
-        <v>20935</v>
+        <f t="shared" si="8"/>
+        <v>33962</v>
       </c>
       <c r="G29" s="5">
         <v>0.1</v>
@@ -1633,11 +1628,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I29" s="1">
-        <v>30025</v>
+        <v>42000</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="10"/>
-        <v>35325</v>
+        <f t="shared" si="11"/>
+        <v>49413</v>
       </c>
       <c r="K29" s="1">
         <v>2757</v>
@@ -1645,23 +1640,23 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B30" t="b">
         <v>0</v>
       </c>
       <c r="C30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>25299</v>
+        <v>17309</v>
       </c>
       <c r="F30" s="1">
-        <f t="shared" si="7"/>
-        <v>29765</v>
+        <f t="shared" si="8"/>
+        <v>20365</v>
       </c>
       <c r="G30" s="5">
         <v>0.1</v>
@@ -1670,35 +1665,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I30" s="1">
-        <v>42000</v>
+        <v>29207</v>
       </c>
       <c r="J30" s="1">
-        <f t="shared" si="10"/>
-        <v>49413</v>
+        <f t="shared" si="11"/>
+        <v>34362</v>
       </c>
       <c r="K30" s="1">
-        <v>2757</v>
+        <v>2682</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E31" s="1">
-        <v>28867</v>
+        <v>22922</v>
       </c>
       <c r="F31" s="1">
-        <f t="shared" si="7"/>
-        <v>33962</v>
+        <f t="shared" si="8"/>
+        <v>26968</v>
       </c>
       <c r="G31" s="5">
         <v>0.1</v>
@@ -1707,14 +1702,14 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I31" s="1">
-        <v>42000</v>
+        <v>33500</v>
       </c>
       <c r="J31" s="1">
-        <f t="shared" si="10"/>
-        <v>49413</v>
+        <f t="shared" si="11"/>
+        <v>39413</v>
       </c>
       <c r="K31" s="1">
-        <v>2757</v>
+        <v>2682</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
@@ -1722,20 +1717,20 @@
         <v>11</v>
       </c>
       <c r="B32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>
       </c>
       <c r="D32" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32" s="1">
-        <v>17309</v>
+        <v>25867</v>
       </c>
       <c r="F32" s="1">
-        <f t="shared" si="7"/>
-        <v>20365</v>
+        <f t="shared" si="8"/>
+        <v>30433</v>
       </c>
       <c r="G32" s="5">
         <v>0.1</v>
@@ -1744,11 +1739,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I32" s="1">
-        <v>29207</v>
+        <v>33500</v>
       </c>
       <c r="J32" s="1">
-        <f t="shared" si="10"/>
-        <v>34362</v>
+        <f t="shared" si="11"/>
+        <v>39413</v>
       </c>
       <c r="K32" s="1">
         <v>2682</v>
@@ -1756,23 +1751,23 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B33" t="b">
         <v>0</v>
       </c>
       <c r="C33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
       </c>
       <c r="E33" s="1">
-        <v>22922</v>
+        <v>16740</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="7"/>
-        <v>26968</v>
+        <f t="shared" si="8"/>
+        <v>19695</v>
       </c>
       <c r="G33" s="5">
         <v>0.1</v>
@@ -1781,35 +1776,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I33" s="1">
-        <v>33500</v>
+        <v>28247</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="10"/>
-        <v>39413</v>
+        <f t="shared" si="11"/>
+        <v>33233</v>
       </c>
       <c r="K33" s="1">
-        <v>2682</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>25867</v>
+        <v>21637</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="7"/>
-        <v>30433</v>
+        <f t="shared" si="8"/>
+        <v>25456</v>
       </c>
       <c r="G34" s="5">
         <v>0.1</v>
@@ -1821,11 +1816,11 @@
         <v>33500</v>
       </c>
       <c r="J34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>39413</v>
       </c>
       <c r="K34" s="1">
-        <v>2682</v>
+        <v>2594</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
@@ -1833,20 +1828,20 @@
         <v>12</v>
       </c>
       <c r="B35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C35" t="b">
         <v>0</v>
       </c>
       <c r="D35" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="1">
-        <v>16740</v>
+        <v>24867</v>
       </c>
       <c r="F35" s="1">
-        <f t="shared" si="7"/>
-        <v>19695</v>
+        <f t="shared" si="8"/>
+        <v>29256</v>
       </c>
       <c r="G35" s="5">
         <v>0.1</v>
@@ -1855,11 +1850,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I35" s="1">
-        <v>28247</v>
+        <v>33500</v>
       </c>
       <c r="J35" s="1">
-        <f t="shared" si="10"/>
-        <v>33233</v>
+        <f t="shared" si="11"/>
+        <v>39413</v>
       </c>
       <c r="K35" s="1">
         <v>2594</v>
@@ -1867,44 +1862,44 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B36" t="b">
         <v>0</v>
       </c>
       <c r="C36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D36" t="b">
         <v>0</v>
       </c>
       <c r="E36" s="1">
-        <v>21637</v>
+        <v>16284</v>
       </c>
       <c r="F36" s="1">
-        <f t="shared" si="7"/>
-        <v>25456</v>
+        <f t="shared" si="8"/>
+        <v>17605</v>
       </c>
       <c r="G36" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H36" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I36" s="1">
-        <v>33500</v>
+        <v>27478</v>
       </c>
       <c r="J36" s="1">
-        <f t="shared" si="10"/>
-        <v>39413</v>
+        <f t="shared" si="11"/>
+        <v>29707</v>
       </c>
       <c r="K36" s="1">
-        <v>2594</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B37" t="b">
         <v>1</v>
@@ -1916,27 +1911,27 @@
         <v>1</v>
       </c>
       <c r="E37" s="1">
-        <v>24867</v>
+        <v>21968</v>
       </c>
       <c r="F37" s="1">
-        <f t="shared" si="7"/>
-        <v>29256</v>
+        <f t="shared" si="8"/>
+        <v>23750</v>
       </c>
       <c r="G37" s="5">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H37" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I37" s="1">
-        <v>33500</v>
+        <v>31729</v>
       </c>
       <c r="J37" s="1">
-        <f t="shared" si="10"/>
-        <v>39413</v>
+        <f t="shared" si="11"/>
+        <v>34303</v>
       </c>
       <c r="K37" s="1">
-        <v>2594</v>
+        <v>2523</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -1947,17 +1942,17 @@
         <v>0</v>
       </c>
       <c r="C38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" t="b">
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <v>16284</v>
+        <v>19583</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="7"/>
-        <v>17605</v>
+        <f t="shared" si="8"/>
+        <v>21172</v>
       </c>
       <c r="G38" s="5">
         <v>0.2</v>
@@ -1966,11 +1961,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I38" s="1">
-        <v>27478</v>
+        <v>31729</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="10"/>
-        <v>29707</v>
+        <f t="shared" si="11"/>
+        <v>34303</v>
       </c>
       <c r="K38" s="1">
         <v>2523</v>
@@ -1978,23 +1973,23 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C39" t="b">
         <v>0</v>
       </c>
       <c r="D39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E39" s="1">
-        <v>21968</v>
+        <v>15902</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="7"/>
-        <v>23750</v>
+        <f t="shared" si="8"/>
+        <v>17192</v>
       </c>
       <c r="G39" s="5">
         <v>0.2</v>
@@ -2003,35 +1998,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I39" s="1">
-        <v>31729</v>
+        <v>26834</v>
       </c>
       <c r="J39" s="1">
-        <f t="shared" si="10"/>
-        <v>34303</v>
+        <f t="shared" si="11"/>
+        <v>29011</v>
       </c>
       <c r="K39" s="1">
-        <v>2523</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C40" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D40" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="1">
-        <v>19583</v>
+        <v>20500</v>
       </c>
       <c r="F40" s="1">
-        <f t="shared" si="7"/>
-        <v>21172</v>
+        <f t="shared" si="8"/>
+        <v>22163</v>
       </c>
       <c r="G40" s="5">
         <v>0.2</v>
@@ -2043,11 +2038,11 @@
         <v>31729</v>
       </c>
       <c r="J40" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>34303</v>
       </c>
       <c r="K40" s="1">
-        <v>2523</v>
+        <v>2464</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -2058,17 +2053,17 @@
         <v>0</v>
       </c>
       <c r="C41" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
       <c r="E41" s="1">
-        <v>15902</v>
+        <v>19252</v>
       </c>
       <c r="F41" s="1">
-        <f t="shared" si="7"/>
-        <v>17192</v>
+        <f t="shared" si="8"/>
+        <v>20814</v>
       </c>
       <c r="G41" s="5">
         <v>0.2</v>
@@ -2077,11 +2072,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I41" s="1">
-        <v>26834</v>
+        <v>31729</v>
       </c>
       <c r="J41" s="1">
-        <f t="shared" si="10"/>
-        <v>29011</v>
+        <f t="shared" si="11"/>
+        <v>34303</v>
       </c>
       <c r="K41" s="1">
         <v>2464</v>
@@ -2089,23 +2084,23 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C42" t="b">
         <v>0</v>
       </c>
       <c r="D42" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42" s="1">
-        <v>20500</v>
+        <v>15529</v>
       </c>
       <c r="F42" s="1">
-        <f t="shared" si="7"/>
-        <v>22163</v>
+        <f t="shared" si="8"/>
+        <v>16789</v>
       </c>
       <c r="G42" s="5">
         <v>0.2</v>
@@ -2114,35 +2109,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I42" s="1">
-        <v>31729</v>
+        <v>26205</v>
       </c>
       <c r="J42" s="1">
-        <f t="shared" si="10"/>
-        <v>34303</v>
+        <f t="shared" si="11"/>
+        <v>28331</v>
       </c>
       <c r="K42" s="1">
-        <v>2464</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43" s="1">
-        <v>19252</v>
+        <v>20500</v>
       </c>
       <c r="F43" s="1">
-        <f t="shared" si="7"/>
-        <v>20814</v>
+        <f t="shared" si="8"/>
+        <v>22163</v>
       </c>
       <c r="G43" s="5">
         <v>0.2</v>
@@ -2154,11 +2149,11 @@
         <v>31729</v>
       </c>
       <c r="J43" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>34303</v>
       </c>
       <c r="K43" s="1">
-        <v>2464</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -2169,17 +2164,17 @@
         <v>0</v>
       </c>
       <c r="C44" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" t="b">
         <v>0</v>
       </c>
       <c r="E44" s="1">
-        <v>15529</v>
+        <v>18141</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" si="7"/>
-        <v>16789</v>
+        <f t="shared" si="8"/>
+        <v>19613</v>
       </c>
       <c r="G44" s="5">
         <v>0.2</v>
@@ -2188,11 +2183,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I44" s="1">
-        <v>26205</v>
+        <v>31729</v>
       </c>
       <c r="J44" s="1">
-        <f t="shared" si="10"/>
-        <v>28331</v>
+        <f t="shared" si="11"/>
+        <v>34303</v>
       </c>
       <c r="K44" s="1">
         <v>2406</v>
@@ -2200,23 +2195,23 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C45" t="b">
         <v>0</v>
       </c>
       <c r="D45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" s="1">
-        <v>20500</v>
+        <v>15062</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" si="7"/>
-        <v>22163</v>
+        <f t="shared" si="8"/>
+        <v>16284</v>
       </c>
       <c r="G45" s="5">
         <v>0.2</v>
@@ -2225,35 +2220,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I45" s="1">
-        <v>31729</v>
+        <v>25417</v>
       </c>
       <c r="J45" s="1">
-        <f t="shared" si="10"/>
-        <v>34303</v>
+        <f t="shared" si="11"/>
+        <v>27479</v>
       </c>
       <c r="K45" s="1">
-        <v>2406</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="1">
-        <v>18141</v>
+        <v>20000</v>
       </c>
       <c r="F46" s="1">
-        <f t="shared" si="7"/>
-        <v>19613</v>
+        <f t="shared" ref="F46:F60" si="12">ROUND((E46 +1)*G46/(G46-H46), 0)</f>
+        <v>21623</v>
       </c>
       <c r="G46" s="5">
         <v>0.2</v>
@@ -2265,11 +2260,11 @@
         <v>31729</v>
       </c>
       <c r="J46" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>34303</v>
       </c>
       <c r="K46" s="1">
-        <v>2406</v>
+        <v>2334</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -2280,17 +2275,17 @@
         <v>0</v>
       </c>
       <c r="C47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" t="b">
         <v>0</v>
       </c>
       <c r="E47" s="1">
-        <v>15062</v>
+        <v>17164</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="7"/>
-        <v>16284</v>
+        <f t="shared" si="12"/>
+        <v>18557</v>
       </c>
       <c r="G47" s="5">
         <v>0.2</v>
@@ -2299,11 +2294,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I47" s="1">
-        <v>25417</v>
+        <v>31729</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="10"/>
-        <v>27479</v>
+        <f t="shared" si="11"/>
+        <v>34303</v>
       </c>
       <c r="K47" s="1">
         <v>2334</v>
@@ -2311,23 +2306,23 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C48" t="b">
         <v>0</v>
       </c>
       <c r="D48" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48" s="1">
-        <v>20000</v>
+        <v>14539</v>
       </c>
       <c r="F48" s="1">
-        <f t="shared" ref="F48:F62" si="11">ROUND((E48 +1)*G48/(G48-H48), 0)</f>
-        <v>21623</v>
+        <f t="shared" si="12"/>
+        <v>15719</v>
       </c>
       <c r="G48" s="5">
         <v>0.2</v>
@@ -2336,35 +2331,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I48" s="1">
-        <v>31729</v>
+        <v>24534</v>
       </c>
       <c r="J48" s="1">
-        <f t="shared" si="10"/>
-        <v>34303</v>
+        <f t="shared" si="11"/>
+        <v>26524</v>
       </c>
       <c r="K48" s="1">
-        <v>2334</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49" s="1">
-        <v>17164</v>
+        <v>20000</v>
       </c>
       <c r="F49" s="1">
-        <f t="shared" si="11"/>
-        <v>18557</v>
+        <f t="shared" si="12"/>
+        <v>21623</v>
       </c>
       <c r="G49" s="5">
         <v>0.2</v>
@@ -2376,11 +2371,11 @@
         <v>31729</v>
       </c>
       <c r="J49" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>34303</v>
       </c>
       <c r="K49" s="1">
-        <v>2334</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
@@ -2391,17 +2386,17 @@
         <v>0</v>
       </c>
       <c r="C50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" t="b">
         <v>0</v>
       </c>
       <c r="E50" s="1">
-        <v>14539</v>
+        <v>16570</v>
       </c>
       <c r="F50" s="1">
-        <f t="shared" si="11"/>
-        <v>15719</v>
+        <f t="shared" si="12"/>
+        <v>17915</v>
       </c>
       <c r="G50" s="5">
         <v>0.2</v>
@@ -2410,11 +2405,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I50" s="1">
-        <v>24534</v>
+        <v>31729</v>
       </c>
       <c r="J50" s="1">
-        <f t="shared" si="10"/>
-        <v>26524</v>
+        <f t="shared" si="11"/>
+        <v>34303</v>
       </c>
       <c r="K50" s="1">
         <v>2253</v>
@@ -2422,23 +2417,23 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C51" t="b">
         <v>0</v>
       </c>
       <c r="D51" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51" s="1">
-        <v>20000</v>
+        <v>13807</v>
       </c>
       <c r="F51" s="1">
-        <f t="shared" si="11"/>
-        <v>21623</v>
+        <f t="shared" si="12"/>
+        <v>14928</v>
       </c>
       <c r="G51" s="5">
         <v>0.2</v>
@@ -2447,35 +2442,35 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I51" s="1">
-        <v>31729</v>
+        <v>23300</v>
       </c>
       <c r="J51" s="1">
-        <f t="shared" si="10"/>
-        <v>34303</v>
+        <f t="shared" si="11"/>
+        <v>25190</v>
       </c>
       <c r="K51" s="1">
-        <v>2253</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52" s="1">
-        <v>16570</v>
+        <v>20000</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="11"/>
-        <v>17915</v>
+        <f t="shared" si="12"/>
+        <v>21623</v>
       </c>
       <c r="G52" s="5">
         <v>0.2</v>
@@ -2487,11 +2482,11 @@
         <v>31729</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>34303</v>
       </c>
       <c r="K52" s="1">
-        <v>2253</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
@@ -2502,17 +2497,17 @@
         <v>0</v>
       </c>
       <c r="C53" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" t="b">
         <v>0</v>
       </c>
       <c r="E53" s="1">
-        <v>13807</v>
+        <v>15970</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" si="11"/>
-        <v>14928</v>
+        <f t="shared" si="12"/>
+        <v>17266</v>
       </c>
       <c r="G53" s="5">
         <v>0.2</v>
@@ -2521,11 +2516,11 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="I53" s="1">
-        <v>23300</v>
+        <v>31729</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" si="10"/>
-        <v>25190</v>
+        <f t="shared" si="11"/>
+        <v>34303</v>
       </c>
       <c r="K53" s="1">
         <v>2140</v>
@@ -2533,23 +2528,23 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" t="b">
         <v>0</v>
       </c>
       <c r="D54" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54" s="1">
-        <v>20000</v>
+        <v>13351</v>
       </c>
       <c r="F54" s="1">
-        <f t="shared" si="11"/>
-        <v>21623</v>
+        <f t="shared" si="12"/>
+        <v>14435</v>
       </c>
       <c r="G54" s="5">
         <v>0.2</v>
@@ -2557,52 +2552,32 @@
       <c r="H54" s="3">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I54" s="1">
-        <v>31729</v>
-      </c>
-      <c r="J54" s="1">
-        <f t="shared" si="10"/>
-        <v>34303</v>
-      </c>
-      <c r="K54" s="1">
-        <v>2140</v>
-      </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B55" t="b">
         <v>0</v>
       </c>
       <c r="C55" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D55" t="b">
         <v>0</v>
       </c>
       <c r="E55" s="1">
-        <v>15970</v>
+        <v>22866</v>
       </c>
       <c r="F55" s="1">
-        <f t="shared" si="11"/>
-        <v>17266</v>
+        <f t="shared" si="12"/>
+        <v>24721</v>
       </c>
       <c r="G55" s="5">
         <v>0.2</v>
       </c>
       <c r="H55" s="3">
         <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="I55" s="1">
-        <v>31729</v>
-      </c>
-      <c r="J55" s="1">
-        <f t="shared" si="10"/>
-        <v>34303</v>
-      </c>
-      <c r="K55" s="1">
-        <v>2140</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -2619,11 +2594,11 @@
         <v>0</v>
       </c>
       <c r="E56" s="1">
-        <v>13351</v>
+        <v>24966</v>
       </c>
       <c r="F56" s="1">
-        <f t="shared" si="11"/>
-        <v>14435</v>
+        <f t="shared" si="12"/>
+        <v>26991</v>
       </c>
       <c r="G56" s="5">
         <v>0.2</v>
@@ -2646,11 +2621,11 @@
         <v>0</v>
       </c>
       <c r="E57" s="1">
-        <v>22866</v>
+        <v>24966</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" si="11"/>
-        <v>24721</v>
+        <f t="shared" si="12"/>
+        <v>26991</v>
       </c>
       <c r="G57" s="5">
         <v>0.2</v>
@@ -2672,18 +2647,9 @@
       <c r="D58" t="b">
         <v>0</v>
       </c>
-      <c r="E58" s="1">
-        <v>24966</v>
-      </c>
-      <c r="F58" s="1">
-        <f t="shared" si="11"/>
-        <v>26991</v>
-      </c>
-      <c r="G58" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H58" s="3">
-        <v>1.4999999999999999E-2</v>
+      <c r="F58" s="1" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -2691,26 +2657,17 @@
         <v>34</v>
       </c>
       <c r="B59" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C59" t="b">
         <v>0</v>
       </c>
       <c r="D59" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" s="1">
-        <v>24966</v>
-      </c>
-      <c r="F59" s="1">
-        <f t="shared" si="11"/>
-        <v>26991</v>
-      </c>
-      <c r="G59" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="H59" s="3">
-        <v>1.4999999999999999E-2</v>
+        <v>1</v>
+      </c>
+      <c r="F59" s="1" t="e">
+        <f t="shared" si="12"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -2721,57 +2678,21 @@
         <v>0</v>
       </c>
       <c r="C60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" t="b">
         <v>0</v>
       </c>
       <c r="F60" s="1" t="e">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>34</v>
-      </c>
-      <c r="B61" t="b">
-        <v>1</v>
-      </c>
-      <c r="C61" t="b">
-        <v>0</v>
-      </c>
-      <c r="D61" t="b">
-        <v>1</v>
-      </c>
-      <c r="F61" s="1" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" t="s">
-        <v>34</v>
-      </c>
-      <c r="B62" t="b">
-        <v>0</v>
-      </c>
-      <c r="C62" t="b">
-        <v>1</v>
-      </c>
-      <c r="D62" t="b">
-        <v>0</v>
-      </c>
-      <c r="F62" s="1" t="e">
-        <f t="shared" si="11"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A10:K40">
-    <sortCondition descending="1" ref="A10:A40"/>
-    <sortCondition ref="D10:D40"/>
-    <sortCondition ref="B10:B40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:K38">
+    <sortCondition descending="1" ref="A8:A38"/>
+    <sortCondition ref="D8:D38"/>
+    <sortCondition ref="B8:B38"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3176,10 +3097,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
         <v>43</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>